<commit_message>
Implemented basic OLET handling. Works only if target is a pipe.
</commit_message>
<xml_diff>
--- a/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
+++ b/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>PIPELINE-REFERENCE</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Olet: Weldolet</t>
+  </si>
+  <si>
+    <t>Olet</t>
+  </si>
+  <si>
+    <t>Pipe Types: Stålrør, sømløse, tap</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,6 +580,12 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added valve as adaptive element
</commit_message>
<xml_diff>
--- a/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
+++ b/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\Revit-PCF-Importer\Revit-PCF-Importer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Revit-PCF-Importer\Revit-PCF-Importer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>PIPELINE-REFERENCE</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>FVR</t>
+  </si>
+  <si>
+    <t>GenValve: Std</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +557,9 @@
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -582,6 +588,9 @@
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Handling of PCF valves
</commit_message>
<xml_diff>
--- a/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
+++ b/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Revit-PCF-Importer\Revit-PCF-Importer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\Revit-PCF-Importer\Revit-PCF-Importer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,7 +101,7 @@
     <t>FVR</t>
   </si>
   <si>
-    <t>GenValve: Std</t>
+    <t>GenericPCFValve: Std</t>
   </si>
 </sst>
 </file>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add some null checks
</commit_message>
<xml_diff>
--- a/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
+++ b/Revit-PCF-Importer/PCF_Importer_Configuration.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\Revit-PCF-Importer\Revit-PCF-Importer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\shtirlitsDva\Revit-PCF-Importer\Revit-PCF-Importer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B03E95-A236-415C-B5EA-0019767C8ED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38295" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All pipelines" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>PIPELINE-REFERENCE</t>
   </si>
@@ -102,12 +103,18 @@
   </si>
   <si>
     <t>GenericPCFValve: Std</t>
+  </si>
+  <si>
+    <t>VF</t>
+  </si>
+  <si>
+    <t>VR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -462,11 +469,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +538,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -563,7 +570,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -595,9 +602,73 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>